<commit_message>
WIP standby event handling
</commit_message>
<xml_diff>
--- a/RAB 2024.xlsx
+++ b/RAB 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\C# Projects\EasyBillingService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227B7CFB-BC71-4253-904A-6FE8CE23C68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{211D397B-23C3-44EA-9D97-DA4D537C153C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="49">
   <si>
     <t>Re-Nr.</t>
   </si>
@@ -165,42 +165,6 @@
   </si>
   <si>
     <t>Jahresergebnis 2024</t>
-  </si>
-  <si>
-    <t>Jan 24</t>
-  </si>
-  <si>
-    <t>Feb 24</t>
-  </si>
-  <si>
-    <t>Mrz 24</t>
-  </si>
-  <si>
-    <t>Apr 24</t>
-  </si>
-  <si>
-    <t>Mai 24</t>
-  </si>
-  <si>
-    <t>Jun 24</t>
-  </si>
-  <si>
-    <t>Jul 24</t>
-  </si>
-  <si>
-    <t>Aug 24</t>
-  </si>
-  <si>
-    <t>Sep 24</t>
-  </si>
-  <si>
-    <t>Okt 24</t>
-  </si>
-  <si>
-    <t>Nov 24</t>
-  </si>
-  <si>
-    <t>Dez 24</t>
   </si>
   <si>
     <t>LKBS: Kirchengem. Gittelde</t>
@@ -258,8 +222,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$-407]mmm/\ yy;@"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -369,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -515,21 +480,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -552,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -597,9 +547,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,9 +688,6 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,10 +709,10 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -782,11 +726,14 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1096,11 +1043,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M247"/>
+  <dimension ref="A1:M248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1062,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1123,40 +1070,40 @@
       <c r="A2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
-      <c r="B4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1164,30 +1111,30 @@
       <c r="G4" s="6"/>
       <c r="H4" s="12"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="46"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="A5" s="81">
+        <v>45292</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="6"/>
       <c r="H5" s="12"/>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="49" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="4">
         <v>45321</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2">
         <v>1350</v>
@@ -1195,7 +1142,7 @@
       <c r="E6" s="10">
         <v>1606.5</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="50">
         <f>SUM(E6,-D6)</f>
         <v>256.5</v>
       </c>
@@ -1211,20 +1158,20 @@
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="55" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="55">
         <f>SUM(D6:D6)</f>
         <v>1350</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="55">
         <f>SUM(E6:E6)</f>
         <v>1606.5</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="56">
         <f>SUM(F6:F6)</f>
         <v>256.5</v>
       </c>
@@ -1240,25 +1187,25 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="61"/>
+      <c r="A9" s="81">
+        <v>45323</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="51" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="4">
         <v>45340</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2">
         <v>7891.28</v>
@@ -1267,7 +1214,7 @@
         <f t="shared" ref="E10:E13" si="0">PRODUCT(D10*1.19)</f>
         <v>9390.6232</v>
       </c>
-      <c r="F10" s="51">
+      <c r="F10" s="50">
         <f t="shared" ref="F10:F13" si="1">SUM(E10,-D10)</f>
         <v>1499.3432000000003</v>
       </c>
@@ -1280,14 +1227,14 @@
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
-        <v>46</v>
+      <c r="A11" s="49" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="4">
         <v>45348</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>5000</v>
@@ -1296,26 +1243,26 @@
         <f t="shared" si="0"/>
         <v>5950</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="50">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
-        <v>48</v>
+      <c r="A12" s="51" t="s">
+        <v>36</v>
       </c>
       <c r="B12" s="7">
         <v>45348</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>2634.42</v>
@@ -1324,7 +1271,7 @@
         <f t="shared" si="0"/>
         <v>3134.9598000000001</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="50">
         <f t="shared" si="1"/>
         <v>500.53980000000001</v>
       </c>
@@ -1336,14 +1283,14 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
-        <v>49</v>
+      <c r="A13" s="51" t="s">
+        <v>37</v>
       </c>
       <c r="B13" s="7">
         <v>45349</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2">
         <v>2140</v>
@@ -1352,7 +1299,7 @@
         <f t="shared" si="0"/>
         <v>2546.6</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="50">
         <f t="shared" si="1"/>
         <v>406.59999999999991</v>
       </c>
@@ -1362,20 +1309,20 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="55" t="s">
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="55">
         <f>SUM(D10:D13)</f>
         <v>17665.699999999997</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E14" s="55">
         <f>SUM(E10:E12)</f>
         <v>18475.582999999999</v>
       </c>
-      <c r="F14" s="57">
+      <c r="F14" s="56">
         <f>SUM(F10:F12)</f>
         <v>2949.8830000000003</v>
       </c>
@@ -1391,25 +1338,25 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
+      <c r="A16" s="81">
+        <v>45352</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>51</v>
+      <c r="A17" s="51" t="s">
+        <v>39</v>
       </c>
       <c r="B17" s="7">
         <v>45357</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D17" s="2">
         <v>4201.68</v>
@@ -1417,35 +1364,35 @@
       <c r="E17" s="10">
         <v>5000</v>
       </c>
-      <c r="F17" s="51">
-        <f t="shared" ref="F17:F22" si="2">SUM(E17,-D17)</f>
+      <c r="F17" s="50">
+        <f t="shared" ref="F17:F20" si="2">SUM(E17,-D17)</f>
         <v>798.31999999999971</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
-        <v>53</v>
+      <c r="A18" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="7">
         <v>45357</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2">
         <v>5747.95</v>
       </c>
       <c r="E18" s="10">
-        <f t="shared" ref="E18:E22" si="3">PRODUCT(D18*1.19)</f>
+        <f t="shared" ref="E18:E20" si="3">PRODUCT(D18*1.19)</f>
         <v>6840.0604999999996</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="50">
         <f t="shared" si="2"/>
         <v>1092.1104999999998</v>
       </c>
@@ -1457,14 +1404,14 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
-        <v>56</v>
+      <c r="A19" s="51" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="7">
         <v>45358</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2">
         <v>3192.08</v>
@@ -1473,7 +1420,7 @@
         <f t="shared" si="3"/>
         <v>3798.5751999999998</v>
       </c>
-      <c r="F19" s="51">
+      <c r="F19" s="50">
         <f t="shared" si="2"/>
         <v>606.49519999999984</v>
       </c>
@@ -1485,14 +1432,14 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
-        <v>59</v>
+      <c r="A20" s="51" t="s">
+        <v>47</v>
       </c>
       <c r="B20" s="7">
         <v>45365</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D20" s="2">
         <v>13000</v>
@@ -1501,7 +1448,7 @@
         <f t="shared" si="3"/>
         <v>15470</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="50">
         <f t="shared" si="2"/>
         <v>2470</v>
       </c>
@@ -1513,116 +1460,93 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
+      <c r="A21" s="51">
+        <v>2249009</v>
+      </c>
+      <c r="B21" s="7">
+        <v>45377.388032407405</v>
+      </c>
       <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="51">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>25</v>
-      </c>
+        <v>336212.55</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="51">
+        <v>2249010</v>
+      </c>
+      <c r="B22" s="7">
+        <v>45377.389351851853</v>
+      </c>
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E22" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="51">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="13"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="56">
-        <f>SUM(D17:D20)</f>
-        <v>26141.71</v>
-      </c>
-      <c r="E23" s="56">
-        <f>SUM(E17:E22)</f>
-        <v>31108.635699999999</v>
-      </c>
-      <c r="F23" s="57">
-        <f>SUM(F17:F20)</f>
-        <v>4966.9256999999998</v>
-      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="61"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="2"/>
       <c r="I23" s="13"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="10"/>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="52"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="55">
+        <f>SUM(D17:D20)</f>
+        <v>26141.71</v>
+      </c>
+      <c r="E24" s="55">
+        <f>SUM(E17:E23)</f>
+        <v>31108.635699999999</v>
+      </c>
+      <c r="F24" s="56">
+        <f>SUM(F17:F20)</f>
+        <v>4966.9256999999998</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="I24" s="13"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="4"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="2"/>
+      <c r="I25" s="13"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="61" t="s">
+      <c r="F26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="63"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10">
-        <f t="shared" ref="E27:E32" si="4">PRODUCT(D27*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="51">
-        <f t="shared" ref="F27:F32" si="5">SUM(E27,-D27)</f>
-        <v>0</v>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="81">
+        <v>45383</v>
+      </c>
+      <c r="B27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="60" t="s">
+        <v>26</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="13" t="s">
@@ -1630,18 +1554,18 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="4"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="E28:E33" si="4">PRODUCT(D28*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="50">
+        <f t="shared" ref="F28:F33" si="5">SUM(E28,-D28)</f>
         <v>0</v>
       </c>
       <c r="G28" s="4"/>
@@ -1650,7 +1574,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="63"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="4"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2">
@@ -1660,7 +1584,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F29" s="51">
+      <c r="F29" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1670,7 +1594,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="4"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2">
@@ -1680,19 +1604,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F30" s="51">
+      <c r="F30" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="2">
         <v>0</v>
       </c>
@@ -1700,7 +1624,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F31" s="51">
+      <c r="F31" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1712,9 +1636,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="1"/>
+      <c r="A32" s="51"/>
       <c r="D32" s="2">
         <v>0</v>
       </c>
@@ -1722,7 +1644,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F32" s="51">
+      <c r="F32" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1733,106 +1655,100 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="64"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="55" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="49"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="63"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="56">
-        <f>SUM(D30:D32)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="56">
-        <f>SUM(E30:E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="57">
-        <f>SUM(F30:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="D34" s="55">
+        <f>SUM(D31:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="55">
+        <f>SUM(E31:E33)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="56">
+        <f>SUM(F31:F33)</f>
+        <v>0</v>
+      </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="4"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="14"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="F35" s="8"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="61" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="10">
-        <f t="shared" ref="E37:E42" si="6">PRODUCT(D37*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="51">
-        <f t="shared" ref="F37:F42" si="7">SUM(E37,-D37)</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>25</v>
-      </c>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="81">
+        <v>45413</v>
+      </c>
+      <c r="B37" s="57"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="A38" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
       </c>
       <c r="E38" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E38:E43" si="6">PRODUCT(D38*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="50">
+        <f t="shared" ref="F38:F43" si="7">SUM(E38,-D38)</f>
         <v>0</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -1843,7 +1759,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="50" t="s">
+      <c r="A39" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -1859,7 +1775,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F39" s="51">
+      <c r="F39" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -1871,7 +1787,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -1887,7 +1803,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F40" s="51">
+      <c r="F40" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -1899,7 +1815,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1915,7 +1831,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F41" s="51">
+      <c r="F41" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -1927,9 +1843,15 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="1"/>
+      <c r="A42" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D42" s="2">
         <v>0</v>
       </c>
@@ -1937,100 +1859,104 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F42" s="51">
+      <c r="F42" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H42" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="64"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="55" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="49"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="50">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="63"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="56">
-        <f>SUM(D40:D42)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="56">
-        <f>SUM(E40:E42)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="57">
-        <f>SUM(F40:F42)</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
+      <c r="D44" s="55">
+        <f>SUM(D41:D43)</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="55">
+        <f>SUM(E41:E43)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="56">
+        <f>SUM(F41:F43)</f>
+        <v>0</v>
+      </c>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="43"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="14"/>
-      <c r="F45" s="2"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="61" t="s">
-        <v>26</v>
-      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="14"/>
+      <c r="F46" s="2"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="2">
-        <v>0</v>
-      </c>
-      <c r="E47" s="10">
-        <f t="shared" ref="E47:E52" si="8">PRODUCT(D47*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="51">
-        <f t="shared" ref="F47:F52" si="9">SUM(E47,-D47)</f>
-        <v>0</v>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="81">
+        <v>45444</v>
+      </c>
+      <c r="B47" s="57"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="60" t="s">
+        <v>26</v>
       </c>
       <c r="G47" s="4"/>
-      <c r="H47" s="13" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="52"/>
+      <c r="A48" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D48" s="2">
         <v>0</v>
       </c>
       <c r="E48" s="10">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="51">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="E48:E53" si="8">PRODUCT(D48*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="50">
+        <f t="shared" ref="F48:F53" si="9">SUM(E48,-D48)</f>
         <v>0</v>
       </c>
       <c r="G48" s="4"/>
@@ -2039,7 +1965,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
+      <c r="A49" s="51"/>
       <c r="D49" s="2">
         <v>0</v>
       </c>
@@ -2047,7 +1973,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F49" s="51">
+      <c r="F49" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2057,7 +1983,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
+      <c r="A50" s="51"/>
       <c r="D50" s="2">
         <v>0</v>
       </c>
@@ -2065,7 +1991,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F50" s="51">
+      <c r="F50" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2075,7 +2001,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="52"/>
+      <c r="A51" s="51"/>
       <c r="D51" s="2">
         <v>0</v>
       </c>
@@ -2083,7 +2009,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F51" s="51">
+      <c r="F51" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2093,7 +2019,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
+      <c r="A52" s="51"/>
       <c r="D52" s="2">
         <v>0</v>
       </c>
@@ -2101,7 +2027,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F52" s="51">
+      <c r="F52" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2110,87 +2036,77 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="53"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="55" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="51"/>
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+      <c r="E53" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="50">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="52"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="56">
-        <f>SUM(D48:D52)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="56">
-        <f>SUM(E47:E52)</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="57">
-        <f>SUM(F47,F47)</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="D54" s="55">
+        <f>SUM(D49:D53)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="55">
+        <f>SUM(E48:E53)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="56">
+        <f>SUM(F48,F48)</f>
+        <v>0</v>
+      </c>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="4"/>
       <c r="C55" s="14"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
-      <c r="F55" s="2"/>
+      <c r="F55" s="8"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56" s="58"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="68"/>
-      <c r="E56" s="68"/>
-      <c r="F56" s="61" t="s">
-        <v>26</v>
-      </c>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="2"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D57" s="2">
-        <v>0</v>
-      </c>
-      <c r="E57" s="10">
-        <f t="shared" ref="E57:E62" si="10">PRODUCT(D57*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="51">
-        <f t="shared" ref="F57:F62" si="11">SUM(E57,-D57)</f>
-        <v>0</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>25</v>
-      </c>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="81">
+        <v>45474</v>
+      </c>
+      <c r="B57" s="57"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="50" t="s">
+      <c r="A58" s="51" t="s">
         <v>26</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -2203,11 +2119,11 @@
         <v>0</v>
       </c>
       <c r="E58" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F58" s="51">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="E58:E63" si="10">PRODUCT(D58*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="50">
+        <f t="shared" ref="F58:F63" si="11">SUM(E58,-D58)</f>
         <v>0</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -2218,8 +2134,15 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="50"/>
-      <c r="B59" s="9"/>
+      <c r="A59" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D59" s="2">
         <v>0</v>
       </c>
@@ -2227,17 +2150,19 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F59" s="51">
+      <c r="F59" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H59" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="50"/>
+      <c r="A60" s="49"/>
       <c r="B60" s="9"/>
       <c r="D60" s="2">
         <v>0</v>
@@ -2246,7 +2171,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F60" s="51">
+      <c r="F60" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -2256,15 +2181,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A61" s="49"/>
+      <c r="B61" s="9"/>
       <c r="D61" s="2">
         <v>0</v>
       </c>
@@ -2272,19 +2190,17 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F61" s="51">
+      <c r="F61" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G61" s="4"/>
       <c r="H61" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B62" s="9" t="s">
@@ -2300,98 +2216,106 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F62" s="51">
+      <c r="F62" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G62" s="4"/>
+      <c r="G62" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H62" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="69"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="55" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="50">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="H63" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="67"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="56">
-        <f>SUM(D57:D61)</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="56">
-        <f>SUM(E57:E61)</f>
-        <v>0</v>
-      </c>
-      <c r="F63" s="57">
-        <f>SUM(F57:F61)</f>
-        <v>0</v>
-      </c>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="43"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
+      <c r="D64" s="55">
+        <f>SUM(D58:D62)</f>
+        <v>0</v>
+      </c>
+      <c r="E64" s="55">
+        <f>SUM(E58:E62)</f>
+        <v>0</v>
+      </c>
+      <c r="F64" s="56">
+        <f>SUM(F58:F62)</f>
+        <v>0</v>
+      </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
-      <c r="B65" s="4"/>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="42"/>
       <c r="C65" s="14"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="2"/>
+      <c r="F65" s="8"/>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B66" s="58"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="61" t="s">
-        <v>26</v>
-      </c>
+      <c r="A66" s="9"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="2"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="63"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="2">
-        <v>0</v>
-      </c>
-      <c r="E67" s="10">
-        <f t="shared" ref="E67:E72" si="12">PRODUCT(D67*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="51">
-        <f t="shared" ref="F67:F72" si="13">SUM(E67,-D67)</f>
-        <v>0</v>
+    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="81">
+        <v>45505</v>
+      </c>
+      <c r="B67" s="57"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="66"/>
+      <c r="F67" s="60" t="s">
+        <v>26</v>
       </c>
       <c r="G67" s="1"/>
-      <c r="H67" s="13" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="63"/>
+      <c r="A68" s="62"/>
       <c r="B68" s="4"/>
       <c r="C68" s="14"/>
       <c r="D68" s="2">
         <v>0</v>
       </c>
       <c r="E68" s="10">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="F68" s="51">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="E68:E73" si="12">PRODUCT(D68*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F68" s="50">
+        <f t="shared" ref="F68:F73" si="13">SUM(E68,-D68)</f>
         <v>0</v>
       </c>
       <c r="G68" s="1"/>
@@ -2400,7 +2324,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="63"/>
+      <c r="A69" s="62"/>
       <c r="B69" s="4"/>
       <c r="C69" s="14"/>
       <c r="D69" s="2">
@@ -2410,7 +2334,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="F69" s="51">
+      <c r="F69" s="50">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2420,15 +2344,9 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A70" s="62"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="14"/>
       <c r="D70" s="2">
         <v>0</v>
       </c>
@@ -2436,26 +2354,23 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="F70" s="51">
+      <c r="F70" s="50">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G70" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G70" s="1"/>
       <c r="H70" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="7"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="A71" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D71" s="2">
@@ -2465,7 +2380,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="F71" s="51">
+      <c r="F71" s="50">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2475,11 +2390,18 @@
       <c r="H71" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="J71" s="7"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="50"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="1"/>
+      <c r="A72" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D72" s="2">
         <v>0</v>
       </c>
@@ -2487,7 +2409,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="F72" s="51">
+      <c r="F72" s="50">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2497,102 +2419,103 @@
       <c r="H72" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="53"/>
-      <c r="B73" s="54"/>
-      <c r="C73" s="55" t="s">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="49"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+      <c r="E73" s="10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="50">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="52"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D73" s="56">
-        <f>SUM(D70:D72)</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="56">
-        <f>SUM(E70:E72)</f>
-        <v>0</v>
-      </c>
-      <c r="F73" s="57">
-        <f>SUM(F70:F72)</f>
-        <v>0</v>
-      </c>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
+      <c r="D74" s="55">
+        <f>SUM(D71:D73)</f>
+        <v>0</v>
+      </c>
+      <c r="E74" s="55">
+        <f>SUM(E71:E73)</f>
+        <v>0</v>
+      </c>
+      <c r="F74" s="56">
+        <f>SUM(F71:F73)</f>
+        <v>0</v>
+      </c>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
       <c r="B75" s="4"/>
       <c r="C75" s="14"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
-      <c r="F75" s="2"/>
+      <c r="F75" s="8"/>
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B76" s="58"/>
-      <c r="C76" s="67"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="61" t="s">
-        <v>26</v>
-      </c>
+      <c r="A76" s="9"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="2"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="63"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="2">
-        <v>0</v>
-      </c>
-      <c r="E77" s="10">
-        <f t="shared" ref="E77:E82" si="14">PRODUCT(D77*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F77" s="51">
-        <f t="shared" ref="F77:F82" si="15">SUM(E77,-D77)</f>
-        <v>0</v>
+    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="81">
+        <v>45536</v>
+      </c>
+      <c r="B77" s="57"/>
+      <c r="C77" s="65"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="60" t="s">
+        <v>26</v>
       </c>
       <c r="G77" s="1"/>
-      <c r="H77" s="13" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="63"/>
+      <c r="A78" s="62"/>
       <c r="B78" s="4"/>
       <c r="C78" s="14"/>
       <c r="D78" s="2">
         <v>0</v>
       </c>
       <c r="E78" s="10">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F78" s="51">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="E78:E83" si="14">PRODUCT(D78*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F78" s="50">
+        <f t="shared" ref="F78:F83" si="15">SUM(E78,-D78)</f>
         <v>0</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I78" s="27"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="63"/>
+      <c r="A79" s="62"/>
       <c r="B79" s="4"/>
       <c r="C79" s="14"/>
       <c r="D79" s="2">
@@ -2602,7 +2525,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F79" s="51">
+      <c r="F79" s="50">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -2610,11 +2533,12 @@
       <c r="H79" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="I79" s="26"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="70"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="35"/>
+      <c r="A80" s="62"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="14"/>
       <c r="D80" s="2">
         <v>0</v>
       </c>
@@ -2622,20 +2546,19 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F80" s="51">
+      <c r="F80" s="50">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G80" s="4"/>
+      <c r="G80" s="1"/>
       <c r="H80" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J80" s="7"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="71"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="41"/>
+      <c r="A81" s="68"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="34"/>
       <c r="D81" s="2">
         <v>0</v>
       </c>
@@ -2643,21 +2566,20 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F81" s="51">
+      <c r="F81" s="50">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G81" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G81" s="4"/>
       <c r="H81" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="J81" s="7"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="71"/>
-      <c r="B82" s="40"/>
-      <c r="C82" s="41"/>
+      <c r="A82" s="69"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="40"/>
       <c r="D82" s="2">
         <v>0</v>
       </c>
@@ -2665,7 +2587,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F82" s="51">
+      <c r="F82" s="50">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -2676,104 +2598,105 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="53"/>
-      <c r="B83" s="54"/>
-      <c r="C83" s="55" t="s">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="69"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="2">
+        <v>0</v>
+      </c>
+      <c r="E83" s="10">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="50">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="52"/>
+      <c r="B84" s="53"/>
+      <c r="C84" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D83" s="56">
-        <f>SUM(D80:D82)</f>
-        <v>0</v>
-      </c>
-      <c r="E83" s="56">
-        <f>SUM(E80:E82)</f>
-        <v>0</v>
-      </c>
-      <c r="F83" s="57">
-        <f>SUM(F80:F82)</f>
-        <v>0</v>
-      </c>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
+      <c r="D84" s="55">
+        <f>SUM(D81:D83)</f>
+        <v>0</v>
+      </c>
+      <c r="E84" s="55">
+        <f>SUM(E81:E83)</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="56">
+        <f>SUM(F81:F83)</f>
+        <v>0</v>
+      </c>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="B85" s="4"/>
       <c r="C85" s="14"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="8"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="9"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B86" s="58"/>
-      <c r="C86" s="59"/>
-      <c r="D86" s="60"/>
-      <c r="E86" s="60"/>
-      <c r="F86" s="61" t="s">
-        <v>26</v>
-      </c>
       <c r="G86" s="1"/>
-      <c r="I86" s="25"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="63"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="2">
-        <v>0</v>
-      </c>
-      <c r="E87" s="10">
-        <f t="shared" ref="E87:E92" si="16">PRODUCT(D87*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F87" s="51">
-        <f t="shared" ref="F87:F92" si="17">SUM(E87,-D87)</f>
-        <v>0</v>
+    </row>
+    <row r="87" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="81">
+        <v>45566</v>
+      </c>
+      <c r="B87" s="57"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="59"/>
+      <c r="E87" s="59"/>
+      <c r="F87" s="60" t="s">
+        <v>26</v>
       </c>
       <c r="G87" s="1"/>
-      <c r="H87" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I87" s="25"/>
+      <c r="I87" s="24"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="63"/>
+      <c r="A88" s="62"/>
       <c r="B88" s="4"/>
       <c r="C88" s="1"/>
       <c r="D88" s="2">
         <v>0</v>
       </c>
       <c r="E88" s="10">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="F88" s="51">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="E88:E93" si="16">PRODUCT(D88*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F88" s="50">
+        <f t="shared" ref="F88:F93" si="17">SUM(E88,-D88)</f>
         <v>0</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I88" s="25"/>
+      <c r="I88" s="24"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="63"/>
+      <c r="A89" s="62"/>
       <c r="B89" s="4"/>
       <c r="C89" s="1"/>
       <c r="D89" s="2">
@@ -2783,7 +2706,7 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F89" s="51">
+      <c r="F89" s="50">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2791,18 +2714,12 @@
       <c r="H89" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I89" s="25"/>
+      <c r="I89" s="24"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C90" s="30" t="s">
-        <v>26</v>
-      </c>
+      <c r="A90" s="62"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="1"/>
       <c r="D90" s="2">
         <v>0</v>
       </c>
@@ -2810,25 +2727,24 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F90" s="51">
+      <c r="F90" s="50">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="G90" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G90" s="1"/>
       <c r="H90" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="I90" s="24"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C91" s="31" t="s">
+      <c r="A91" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D91" s="2">
@@ -2838,7 +2754,7 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F91" s="51">
+      <c r="F91" s="50">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2848,19 +2764,15 @@
       <c r="H91" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J91" s="83"/>
-      <c r="K91" s="84"/>
-      <c r="L91" s="84"/>
-      <c r="M91" s="84"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C92" s="33" t="s">
+      <c r="A92" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D92" s="2">
@@ -2870,7 +2782,7 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F92" s="51">
+      <c r="F92" s="50">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2880,93 +2792,97 @@
       <c r="H92" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I92" s="25"/>
-    </row>
-    <row r="93" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="53"/>
-      <c r="B93" s="54"/>
-      <c r="C93" s="55" t="s">
+      <c r="J92" s="82"/>
+      <c r="K92" s="83"/>
+      <c r="L92" s="83"/>
+      <c r="M92" s="83"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0</v>
+      </c>
+      <c r="E93" s="10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F93" s="50">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I93" s="24"/>
+    </row>
+    <row r="94" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="52"/>
+      <c r="B94" s="53"/>
+      <c r="C94" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D93" s="56">
-        <f>SUM(D86:D92)</f>
-        <v>0</v>
-      </c>
-      <c r="E93" s="56">
-        <f>SUM(E86:E92)</f>
-        <v>0</v>
-      </c>
-      <c r="F93" s="57">
-        <f>SUM(F86:F92)</f>
-        <v>0</v>
-      </c>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
+      <c r="D94" s="55">
+        <f>SUM(D87:D93)</f>
+        <v>0</v>
+      </c>
+      <c r="E94" s="55">
+        <f>SUM(E87:E93)</f>
+        <v>0</v>
+      </c>
+      <c r="F94" s="56">
+        <f>SUM(F87:F93)</f>
+        <v>0</v>
+      </c>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="9"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B96" s="75"/>
-      <c r="C96" s="76"/>
-      <c r="D96" s="77"/>
-      <c r="E96" s="77"/>
-      <c r="F96" s="78"/>
+      <c r="A96" s="9"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A97" s="79"/>
-      <c r="B97" s="34"/>
-      <c r="C97" s="35"/>
-      <c r="D97" s="2">
-        <v>0</v>
-      </c>
-      <c r="E97" s="10">
-        <f t="shared" ref="E97:E102" si="18">PRODUCT(D97*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F97" s="51">
-        <f t="shared" ref="F97:F102" si="19">SUM(E97,-D97)</f>
-        <v>0</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I97" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J97" s="5" t="s">
-        <v>26</v>
-      </c>
+    <row r="97" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="81">
+        <v>45597</v>
+      </c>
+      <c r="B97" s="73"/>
+      <c r="C97" s="74"/>
+      <c r="D97" s="75"/>
+      <c r="E97" s="75"/>
+      <c r="F97" s="76"/>
+      <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A98" s="80"/>
-      <c r="B98" s="36"/>
-      <c r="C98" s="37"/>
+      <c r="A98" s="77"/>
+      <c r="B98" s="33"/>
+      <c r="C98" s="34"/>
       <c r="D98" s="2">
         <v>0</v>
       </c>
       <c r="E98" s="10">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="F98" s="51">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="E98:E103" si="18">PRODUCT(D98*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F98" s="50">
+        <f t="shared" ref="F98:F103" si="19">SUM(E98,-D98)</f>
         <v>0</v>
       </c>
       <c r="G98" s="4" t="s">
@@ -2975,11 +2891,17 @@
       <c r="H98" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="I98" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A99" s="79"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="39"/>
+      <c r="A99" s="78"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="36"/>
       <c r="D99" s="2">
         <v>0</v>
       </c>
@@ -2987,19 +2909,21 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="F99" s="51">
+      <c r="F99" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="G99" s="4"/>
+      <c r="G99" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H99" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A100" s="80"/>
-      <c r="B100" s="40"/>
-      <c r="C100" s="37"/>
+      <c r="A100" s="77"/>
+      <c r="B100" s="37"/>
+      <c r="C100" s="38"/>
       <c r="D100" s="2">
         <v>0</v>
       </c>
@@ -3007,26 +2931,19 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="F100" s="51">
+      <c r="F100" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="G100" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G100" s="4"/>
       <c r="H100" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I100" s="25"/>
-      <c r="J100" s="83"/>
-      <c r="K100" s="84"/>
-      <c r="L100" s="84"/>
-      <c r="M100" s="84"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A101" s="70"/>
-      <c r="B101" s="38"/>
-      <c r="C101" s="39"/>
+      <c r="A101" s="78"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="36"/>
       <c r="D101" s="2">
         <v>0</v>
       </c>
@@ -3034,7 +2951,7 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="F101" s="51">
+      <c r="F101" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -3044,11 +2961,16 @@
       <c r="H101" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="I101" s="24"/>
+      <c r="J101" s="82"/>
+      <c r="K101" s="83"/>
+      <c r="L101" s="83"/>
+      <c r="M101" s="83"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A102" s="70"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="39"/>
+      <c r="A102" s="68"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="38"/>
       <c r="D102" s="2">
         <v>0</v>
       </c>
@@ -3056,114 +2978,108 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="F102" s="51">
+      <c r="F102" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="G102" s="4"/>
+      <c r="G102" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H102" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="53"/>
-      <c r="B103" s="54"/>
-      <c r="C103" s="55" t="s">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="68"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="2">
+        <v>0</v>
+      </c>
+      <c r="E103" s="10">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F103" s="50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G103" s="4"/>
+      <c r="H103" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="52"/>
+      <c r="B104" s="53"/>
+      <c r="C104" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D103" s="56">
-        <f>SUM(D97:D102)</f>
-        <v>0</v>
-      </c>
-      <c r="E103" s="56">
-        <f>SUM(E97:E102)</f>
-        <v>0</v>
-      </c>
-      <c r="F103" s="57">
-        <f>SUM(F97:F102)</f>
-        <v>0</v>
-      </c>
-      <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A104" s="9"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="14"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
+      <c r="D104" s="55">
+        <f>SUM(D98:D103)</f>
+        <v>0</v>
+      </c>
+      <c r="E104" s="55">
+        <f>SUM(E98:E103)</f>
+        <v>0</v>
+      </c>
+      <c r="F104" s="56">
+        <f>SUM(F98:F103)</f>
+        <v>0</v>
+      </c>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="9"/>
       <c r="B105" s="4"/>
-      <c r="C105" s="1"/>
+      <c r="C105" s="14"/>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
-      <c r="F105" s="2"/>
+      <c r="F105" s="8"/>
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B106" s="81"/>
-      <c r="C106" s="67"/>
-      <c r="D106" s="68"/>
-      <c r="E106" s="68"/>
-      <c r="F106" s="61"/>
+      <c r="A106" s="9"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A107" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="B107" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C107" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D107" s="2">
-        <v>0</v>
-      </c>
-      <c r="E107" s="10">
-        <f t="shared" ref="E107:E112" si="20">PRODUCT(D107*1.19)</f>
-        <v>0</v>
-      </c>
-      <c r="F107" s="51">
-        <f t="shared" ref="F107:F112" si="21">SUM(E107,-D107)</f>
-        <v>0</v>
-      </c>
-      <c r="G107" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>25</v>
-      </c>
+    <row r="107" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="81">
+        <v>45627</v>
+      </c>
+      <c r="B107" s="79"/>
+      <c r="C107" s="65"/>
+      <c r="D107" s="66"/>
+      <c r="E107" s="66"/>
+      <c r="F107" s="60"/>
+      <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A108" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="B108" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C108" s="31" t="s">
+      <c r="A108" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C108" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D108" s="2">
         <v>0</v>
       </c>
       <c r="E108" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="F108" s="51">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="G108" s="4" t="s">
+        <f t="shared" ref="E108:E113" si="20">PRODUCT(D108*1.19)</f>
+        <v>0</v>
+      </c>
+      <c r="F108" s="50">
+        <f t="shared" ref="F108:F113" si="21">SUM(E108,-D108)</f>
+        <v>0</v>
+      </c>
+      <c r="G108" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H108" s="13" t="s">
@@ -3171,10 +3087,10 @@
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A109" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="B109" s="42" t="s">
+      <c r="A109" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="28" t="s">
         <v>26</v>
       </c>
       <c r="C109" s="30" t="s">
@@ -3187,7 +3103,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="F109" s="51">
+      <c r="F109" s="50">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3199,13 +3115,13 @@
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A110" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="B110" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C110" s="30" t="s">
+      <c r="A110" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D110" s="2">
@@ -3215,7 +3131,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="F110" s="51">
+      <c r="F110" s="50">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3227,13 +3143,13 @@
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A111" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="B111" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C111" s="31" t="s">
+      <c r="A111" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D111" s="2">
@@ -3243,23 +3159,25 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="F111" s="51">
+      <c r="F111" s="50">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="G111" s="7"/>
+      <c r="G111" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H111" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A112" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="B112" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C112" s="31" t="s">
+      <c r="A112" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C112" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D112" s="2">
@@ -3269,95 +3187,112 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="F112" s="51">
+      <c r="F112" s="50">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="G112" s="5"/>
+      <c r="G112" s="7"/>
       <c r="H112" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="53"/>
-      <c r="B113" s="54"/>
-      <c r="C113" s="55" t="s">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C113" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0</v>
+      </c>
+      <c r="E113" s="10">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F113" s="50">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G113" s="5"/>
+      <c r="H113" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="52"/>
+      <c r="B114" s="53"/>
+      <c r="C114" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D113" s="56">
-        <f>SUM(D107:D112)</f>
-        <v>0</v>
-      </c>
-      <c r="E113" s="56">
-        <f>SUM(E105:E112)</f>
-        <v>0</v>
-      </c>
-      <c r="F113" s="57">
-        <f>SUM(E113,-D113)</f>
-        <v>0</v>
-      </c>
-      <c r="G113" s="1"/>
-      <c r="K113" t="s">
-        <v>26</v>
-      </c>
-      <c r="L113" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="M113" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A114" s="9"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="2"/>
+      <c r="D114" s="55">
+        <f>SUM(D108:D113)</f>
+        <v>0</v>
+      </c>
+      <c r="E114" s="55">
+        <f>SUM(E106:E113)</f>
+        <v>0</v>
+      </c>
+      <c r="F114" s="56">
+        <f>SUM(E114,-D114)</f>
+        <v>0</v>
+      </c>
       <c r="G114" s="1"/>
-    </row>
-    <row r="115" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K114" t="s">
+        <v>26</v>
+      </c>
+      <c r="L114" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M114" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="9"/>
       <c r="B115" s="4"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E115" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F115" s="19" t="s">
-        <v>23</v>
-      </c>
+      <c r="C115" s="14"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="2"/>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="9"/>
       <c r="B116" s="4"/>
-      <c r="C116" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D116" s="82">
-        <f>SUM(D7,D14,D23,D33,D43,D53,D63,D73,D83,D93,D103,D113)</f>
-        <v>45157.409999999996</v>
-      </c>
-      <c r="E116" s="18">
-        <f>SUM(E7,E14,E23,E33,E43,E53,E63,E73,E83,E93,E103,E113)</f>
-        <v>51190.718699999998</v>
-      </c>
-      <c r="F116" s="18">
-        <f>SUM(F7,F14,F23,F33,F43,F53,F63,F73,F83,F93,F103,F113)</f>
-        <v>8173.3086999999996</v>
+      <c r="C116" s="1"/>
+      <c r="D116" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E116" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F116" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="9"/>
       <c r="B117" s="4"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
+      <c r="C117" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D117" s="80">
+        <f>SUM(D7,D14,D24,D34,D44,D54,D64,D74,D84,D94,D104,D114)</f>
+        <v>45157.409999999996</v>
+      </c>
+      <c r="E117" s="17">
+        <f>SUM(E7,E14,E24,E34,E44,E54,E64,E74,E84,E94,E104,E114)</f>
+        <v>51190.718699999998</v>
+      </c>
+      <c r="F117" s="17">
+        <f>SUM(F7,F14,F24,F34,F44,F54,F64,F74,F84,F94,F104,F114)</f>
+        <v>8173.3086999999996</v>
+      </c>
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -3383,7 +3318,7 @@
       <c r="B120" s="4"/>
       <c r="C120" s="1"/>
       <c r="D120" s="2"/>
-      <c r="E120" s="20"/>
+      <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1"/>
     </row>
@@ -3392,7 +3327,7 @@
       <c r="B121" s="4"/>
       <c r="C121" s="1"/>
       <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
+      <c r="E121" s="19"/>
       <c r="F121" s="2"/>
       <c r="G121" s="1"/>
     </row>
@@ -4462,9 +4397,9 @@
       <c r="A240" s="9"/>
       <c r="B240" s="4"/>
       <c r="C240" s="1"/>
-      <c r="D240" s="3"/>
-      <c r="E240" s="3"/>
-      <c r="F240" s="3"/>
+      <c r="D240" s="2"/>
+      <c r="E240" s="2"/>
+      <c r="F240" s="2"/>
       <c r="G240" s="1"/>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -4480,9 +4415,9 @@
       <c r="A242" s="9"/>
       <c r="B242" s="4"/>
       <c r="C242" s="1"/>
-      <c r="D242" s="1"/>
-      <c r="E242" s="1"/>
-      <c r="F242" s="1"/>
+      <c r="D242" s="3"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
       <c r="G242" s="1"/>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -4530,10 +4465,19 @@
       <c r="F247" s="1"/>
       <c r="G247" s="1"/>
     </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="9"/>
+      <c r="B248" s="4"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="1"/>
+      <c r="E248" s="1"/>
+      <c r="F248" s="1"/>
+      <c r="G248" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J100:M100"/>
-    <mergeCell ref="J91:M91"/>
+    <mergeCell ref="J101:M101"/>
+    <mergeCell ref="J92:M92"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>